<commit_message>
Avance carga masiva trabajadores.
</commit_message>
<xml_diff>
--- a/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Catalogo del formato de carga de informacion externa.xlsx
+++ b/src/app/00078-GestionPlanillas/WebApp/Assets/application/formatos/Catalogo del formato de carga de informacion externa.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUMBERTO-PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00078-DWeb_GestionPlanillas\src\app\00078-GestionPlanillas\WebApp\Assets\application\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433AEC5A-E5EA-4FDA-8B67-F5D105750941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D748AE83-A8A9-4986-9531-751E89A20818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A22229E-7FFA-4F20-BBFA-6FC8C3493951}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="General" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -542,7 +542,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>